<commit_message>
Fix labels.xlsx and prepare for API
</commit_message>
<xml_diff>
--- a/標籤集合.xlsx
+++ b/標籤集合.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koala\OneDrive\Desktop\ML\final_project\ml-final-project-model\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30F9A93-BA2E-4D27-A490-7A7A43728FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="工作表1" sheetId="1" r:id="rId4"/>
+    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -103,9 +112,6 @@
     <t>pork with scrambled eggs(滑蛋豬肉) 25</t>
   </si>
   <si>
-    <t>sauteed pork (醬燒豬肉) 25</t>
-  </si>
-  <si>
     <t>garlic white meat(蒜泥白肉) 25</t>
   </si>
   <si>
@@ -182,22 +188,70 @@
   </si>
   <si>
     <t>cheese pork chops(起司豬排) 25</t>
+  </si>
+  <si>
+    <r>
+      <t>sauteed pork(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>醬燒豬肉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) 25</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -206,36 +260,44 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -425,26 +487,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="2" width="18.25"/>
-    <col customWidth="1" min="3" max="3" width="14.5"/>
-    <col customWidth="1" min="4" max="4" width="35.38"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -472,7 +539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -484,7 +551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -493,228 +560,229 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22">
-      <c r="D22" s="1" t="s">
+    <row r="22" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23">
-      <c r="D23" s="1" t="s">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24">
-      <c r="D24" s="1" t="s">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25">
-      <c r="D25" s="1" t="s">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26">
-      <c r="D26" s="1" t="s">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27">
-      <c r="D27" s="1" t="s">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28">
-      <c r="D28" s="1" t="s">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29">
-      <c r="D29" s="1" t="s">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30">
-      <c r="D30" s="1" t="s">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31">
-      <c r="D31" s="1" t="s">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32">
-      <c r="D32" s="1" t="s">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33">
-      <c r="D33" s="1" t="s">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34">
-      <c r="D34" s="1" t="s">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35">
-      <c r="D35" s="1" t="s">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36">
-      <c r="D36" s="1" t="s">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37">
-      <c r="D37" s="1" t="s">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38">
-      <c r="D38" s="1" t="s">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39">
-      <c r="D39" s="1" t="s">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40">
-      <c r="D40" s="1" t="s">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41">
-      <c r="D41" s="1" t="s">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42">
-      <c r="D42" s="1" t="s">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43">
-      <c r="D43" s="1" t="s">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44">
-      <c r="D44" s="1" t="s">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="45">
-      <c r="D45" s="1" t="s">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46">
-      <c r="D46" s="1" t="s">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="47">
-      <c r="D47" s="1" t="s">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48">
-      <c r="D48" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>